<commit_message>
Changed the temporary password to be auto generated and bulk user update
</commit_message>
<xml_diff>
--- a/admin/public/Bulk User Creation Format.xlsx
+++ b/admin/public/Bulk User Creation Format.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duwa2\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University of Ruhuna\Semester 6\Software Project\Admin\Easy_Coupon-Admin\admin\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9E9038-3DBA-4D27-907E-E615E8F28290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AC63B3-3161-45B2-83DD-65D3A5F711D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Username</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Full Name</t>
   </si>
@@ -42,13 +39,22 @@
     <t>student</t>
   </si>
   <si>
-    <t>canteena</t>
-  </si>
-  <si>
-    <t>canteenb</t>
-  </si>
-  <si>
-    <t>admin</t>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>RegNo</t>
+  </si>
+  <si>
+    <t>EG</t>
+  </si>
+  <si>
+    <t>Abewiikrama A.B.C</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -101,16 +107,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -393,72 +405,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3919</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
     </row>
   </sheetData>
   <dataValidations xWindow="248" yWindow="284" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select the Role" sqref="D2:D6 D8:D11" xr:uid="{39ED9E71-EFBF-4AC3-9779-C1E899D024B9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select the Role" sqref="F2:F49" xr:uid="{39ED9E71-EFBF-4AC3-9779-C1E899D024B9}">
       <formula1>"student, canteena, canteenb, admin"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{DD4F362C-398D-4DD3-8054-7AAC81E333DB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>